<commit_message>
fix for category for maps.
</commit_message>
<xml_diff>
--- a/database/meta/maplet_info_tags.xlsx
+++ b/database/meta/maplet_info_tags.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bukun\AppData\Local\Temp\Mxt105\RemoteFiles\67538_5_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bukun\AppData\Local\Temp\Mxt105\RemoteFiles\67136_3_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33586B5A-01ED-4EE0-AF35-31D80FBDB111}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D5B063-3332-47C7-A658-5FB42751FDCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="maps" sheetId="1" r:id="rId1"/>
+    <sheet name="documents" sheetId="2" r:id="rId2"/>
+    <sheet name="books" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="297">
   <si>
     <t>m</t>
   </si>
@@ -850,6 +850,110 @@
   </si>
   <si>
     <t>农业气候资源</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t24</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2401</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gyhsd</t>
+  </si>
+  <si>
+    <t>约翰斯顿皇家现代地图集</t>
+  </si>
+  <si>
+    <t>t2205</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gmap1933</t>
+  </si>
+  <si>
+    <t>1933年民国时期地图</t>
+  </si>
+  <si>
+    <t>t2207</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gyg_db</t>
+  </si>
+  <si>
+    <t>东北地区</t>
+  </si>
+  <si>
+    <t>gyg_hn</t>
+  </si>
+  <si>
+    <t>华南地区</t>
+  </si>
+  <si>
+    <t>gyg_hz</t>
+  </si>
+  <si>
+    <t>华中地区</t>
+  </si>
+  <si>
+    <t>gyg_hb</t>
+  </si>
+  <si>
+    <t>华北地区</t>
+  </si>
+  <si>
+    <t>gyg_xb</t>
+  </si>
+  <si>
+    <t>西北地区</t>
+  </si>
+  <si>
+    <t>gyg_xn</t>
+  </si>
+  <si>
+    <t>西南地区</t>
+  </si>
+  <si>
+    <t>t2407</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2402</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2403</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2404</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2405</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2406</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>华东地区</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>gyg_hd</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>china_yg</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国行政区划沿革</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -915,7 +1019,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -927,6 +1031,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1310,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1845,137 +1952,253 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B49" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>260</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1" t="s">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D51" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D52" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D51" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D52" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D53" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D55" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="1" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D56" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="2" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>158</v>
       </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63" t="s">
+        <v>295</v>
+      </c>
+      <c r="D63" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E70" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2294,7 +2517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>

</xml_diff>